<commit_message>
finalizacion  vista duo-economico, solucion de errores y finalizacion de index
</commit_message>
<xml_diff>
--- a/relojes.xlsx
+++ b/relojes.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawli\OneDrive\Documentos\GITHUB WORKSPACE\website_reloj\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawli\OneDrive\Documentos\GITHUB WORKSPACE\website_reloj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7555C82-DCB3-4AB8-8DE8-511B65475781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC986958-D21E-497F-B631-21680977D148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{252815FC-D0C9-4BEB-BF5A-C101C806B681}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Relojes Caballero" sheetId="2" r:id="rId1"/>
+    <sheet name="Relojes Dama" sheetId="1" r:id="rId2"/>
+    <sheet name="Relojes Duo" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="234">
   <si>
     <t>c1</t>
   </si>
@@ -640,6 +641,105 @@
   </si>
   <si>
     <t>d32</t>
+  </si>
+  <si>
+    <t>de1</t>
+  </si>
+  <si>
+    <t>Dúo línea económica</t>
+  </si>
+  <si>
+    <t>de2</t>
+  </si>
+  <si>
+    <t>de3</t>
+  </si>
+  <si>
+    <t>de4</t>
+  </si>
+  <si>
+    <t>de5</t>
+  </si>
+  <si>
+    <t>de6</t>
+  </si>
+  <si>
+    <t>de7</t>
+  </si>
+  <si>
+    <t>de8</t>
+  </si>
+  <si>
+    <t>de9</t>
+  </si>
+  <si>
+    <t>de10</t>
+  </si>
+  <si>
+    <t>de11</t>
+  </si>
+  <si>
+    <t>Celeste, Plata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dúo Q&amp;Q original </t>
+  </si>
+  <si>
+    <t>Dúo Casio original</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dúo Q&amp;Q </t>
+  </si>
+  <si>
+    <t>Dúo Q&amp;Q original</t>
+  </si>
+  <si>
+    <t>de12</t>
+  </si>
+  <si>
+    <t>de13</t>
+  </si>
+  <si>
+    <t>de14</t>
+  </si>
+  <si>
+    <t>de15</t>
+  </si>
+  <si>
+    <t>de16</t>
+  </si>
+  <si>
+    <t>de17</t>
+  </si>
+  <si>
+    <t>de18</t>
+  </si>
+  <si>
+    <t>de19</t>
+  </si>
+  <si>
+    <t>de20</t>
+  </si>
+  <si>
+    <t>de21</t>
+  </si>
+  <si>
+    <t>de22</t>
+  </si>
+  <si>
+    <t>de23</t>
+  </si>
+  <si>
+    <t>de24</t>
+  </si>
+  <si>
+    <t>de25</t>
+  </si>
+  <si>
+    <t>de26</t>
+  </si>
+  <si>
+    <t>de27</t>
   </si>
 </sst>
 </file>
@@ -661,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,6 +771,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,9 +808,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,11 +1145,1111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42CD3B6-245E-4DB9-BECC-F8361A7B49A3}">
+  <dimension ref="A1:E77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>1200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>1299</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>1100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>1190</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>1990</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>1190</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>2099</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>2099</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11">
+        <v>1299</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12">
+        <v>1299</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13">
+        <v>1299</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14">
+        <v>890</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15">
+        <v>820</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>1190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17">
+        <v>1190</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18">
+        <v>750</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19">
+        <v>890</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>1090</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21">
+        <v>1250</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22">
+        <v>1260</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23">
+        <v>920</v>
+      </c>
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24">
+        <v>1299</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25">
+        <v>1790</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26">
+        <v>1799</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>1690</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>990</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29">
+        <v>740</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <v>900</v>
+      </c>
+      <c r="E30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31">
+        <v>1290</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>990</v>
+      </c>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33">
+        <v>2099</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34">
+        <v>890</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35">
+        <v>890</v>
+      </c>
+      <c r="E35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36">
+        <v>1600</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>950</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38">
+        <v>990</v>
+      </c>
+      <c r="E38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39">
+        <v>820</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40">
+        <v>900</v>
+      </c>
+      <c r="E40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41">
+        <v>900</v>
+      </c>
+      <c r="E41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42">
+        <v>1490</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43">
+        <v>920</v>
+      </c>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44">
+        <v>1150</v>
+      </c>
+      <c r="E44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45">
+        <v>1150</v>
+      </c>
+      <c r="E45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46">
+        <v>890</v>
+      </c>
+      <c r="E46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47">
+        <v>890</v>
+      </c>
+      <c r="E47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48">
+        <v>990</v>
+      </c>
+      <c r="E48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49">
+        <v>1440</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50">
+        <v>900</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51">
+        <v>1090</v>
+      </c>
+      <c r="E51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52">
+        <v>1190</v>
+      </c>
+      <c r="E52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53">
+        <v>1190</v>
+      </c>
+      <c r="E53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54">
+        <v>990</v>
+      </c>
+      <c r="E54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55">
+        <v>1290</v>
+      </c>
+      <c r="E55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56">
+        <v>900</v>
+      </c>
+      <c r="E56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57">
+        <v>1190</v>
+      </c>
+      <c r="E57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58">
+        <v>740</v>
+      </c>
+      <c r="E58" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59">
+        <v>1200</v>
+      </c>
+      <c r="E59" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C60">
+        <v>1820</v>
+      </c>
+      <c r="E60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61">
+        <v>1190</v>
+      </c>
+      <c r="E61" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62">
+        <v>1190</v>
+      </c>
+      <c r="E62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63">
+        <v>1600</v>
+      </c>
+      <c r="E63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>116</v>
+      </c>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64">
+        <v>1600</v>
+      </c>
+      <c r="E64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>117</v>
+      </c>
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65">
+        <v>1600</v>
+      </c>
+      <c r="E65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66">
+        <v>1799</v>
+      </c>
+      <c r="E66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67">
+        <v>990</v>
+      </c>
+      <c r="E67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68">
+        <v>990</v>
+      </c>
+      <c r="E68" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69">
+        <v>1990</v>
+      </c>
+      <c r="E69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>122</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70">
+        <v>999</v>
+      </c>
+      <c r="E70" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>123</v>
+      </c>
+      <c r="B71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71">
+        <v>999</v>
+      </c>
+      <c r="E71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72">
+        <v>1150</v>
+      </c>
+      <c r="E72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73">
+        <v>1200</v>
+      </c>
+      <c r="E73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74">
+        <v>1150</v>
+      </c>
+      <c r="E74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75">
+        <v>1200</v>
+      </c>
+      <c r="E75" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76">
+        <v>1150</v>
+      </c>
+      <c r="E76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>143</v>
+      </c>
+      <c r="B77" t="s">
+        <v>149</v>
+      </c>
+      <c r="C77">
+        <v>1150</v>
+      </c>
+      <c r="E77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E966F5D-9ADD-4FBF-AFB8-143A580BCB6E}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,19 +2265,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1278,7 +2485,7 @@
         <v>154</v>
       </c>
       <c r="C16">
-        <v>1250</v>
+        <v>1290</v>
       </c>
       <c r="E16" t="s">
         <v>71</v>
@@ -1529,15 +2736,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42CD3B6-245E-4DB9-BECC-F8361A7B49A3}">
-  <dimension ref="A1:E77"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA117F4-D5F1-4BE9-A2A3-0B41B0F4E011}">
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E77"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -1558,1088 +2769,403 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="C2">
-        <v>1200</v>
+        <v>580</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="C3">
-        <v>1299</v>
+        <v>580</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="C4">
-        <v>1100</v>
+        <v>580</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>580</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="C6">
-        <v>1190</v>
+        <v>580</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
       <c r="C7">
-        <v>1990</v>
+        <v>580</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>202</v>
       </c>
       <c r="C8">
-        <v>1190</v>
+        <v>580</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="C9">
-        <v>2099</v>
+        <v>580</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="C10">
-        <v>2099</v>
+        <v>580</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="C11">
-        <v>1299</v>
+        <v>580</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
       <c r="C12">
-        <v>1299</v>
+        <v>690</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>214</v>
       </c>
       <c r="C13">
-        <v>1299</v>
+        <v>1099</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>219</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="C14">
-        <v>890</v>
+        <v>1600</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>220</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C15">
-        <v>820</v>
+        <v>790</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>202</v>
       </c>
       <c r="C16">
-        <v>1190</v>
+        <v>580</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
       <c r="C17">
-        <v>1190</v>
+        <v>999</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="C18">
-        <v>750</v>
+        <v>580</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="C19">
-        <v>890</v>
+        <v>1450</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>215</v>
       </c>
       <c r="C20">
-        <v>1090</v>
+        <v>1600</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>226</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="C21">
-        <v>1250</v>
+        <v>1500</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>227</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>215</v>
       </c>
       <c r="C22">
-        <v>1260</v>
+        <v>2200</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>228</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="C23">
-        <v>920</v>
+        <v>2500</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
       <c r="C24">
-        <v>1299</v>
+        <v>2500</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="C25">
-        <v>1790</v>
+        <v>1800</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>231</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>215</v>
       </c>
       <c r="C26">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>232</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>215</v>
       </c>
       <c r="C27">
-        <v>1690</v>
+        <v>1800</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>233</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>217</v>
       </c>
       <c r="C28">
-        <v>990</v>
+        <v>1290</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29">
-        <v>740</v>
-      </c>
-      <c r="E29" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30">
-        <v>900</v>
-      </c>
-      <c r="E30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31">
-        <v>1290</v>
-      </c>
-      <c r="E31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32">
-        <v>990</v>
-      </c>
-      <c r="E32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33">
-        <v>2099</v>
-      </c>
-      <c r="E33" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34">
-        <v>890</v>
-      </c>
-      <c r="E34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35">
-        <v>890</v>
-      </c>
-      <c r="E35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36">
-        <v>1600</v>
-      </c>
-      <c r="E36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37">
-        <v>950</v>
-      </c>
-      <c r="E37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38">
-        <v>990</v>
-      </c>
-      <c r="E38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39">
-        <v>820</v>
-      </c>
-      <c r="E39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40">
-        <v>900</v>
-      </c>
-      <c r="E40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41">
-        <v>900</v>
-      </c>
-      <c r="E41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42">
-        <v>1490</v>
-      </c>
-      <c r="E42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43">
-        <v>920</v>
-      </c>
-      <c r="E43" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44">
-        <v>1150</v>
-      </c>
-      <c r="E44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" t="s">
-        <v>124</v>
-      </c>
-      <c r="C45">
-        <v>1150</v>
-      </c>
-      <c r="E45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" t="s">
-        <v>125</v>
-      </c>
-      <c r="C46">
-        <v>890</v>
-      </c>
-      <c r="E46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47">
-        <v>890</v>
-      </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48">
-        <v>990</v>
-      </c>
-      <c r="E48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" t="s">
-        <v>128</v>
-      </c>
-      <c r="C49">
-        <v>1440</v>
-      </c>
-      <c r="E49" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50">
-        <v>900</v>
-      </c>
-      <c r="E50" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" t="s">
-        <v>70</v>
-      </c>
-      <c r="C51">
-        <v>1090</v>
-      </c>
-      <c r="E51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52">
-        <v>1190</v>
-      </c>
-      <c r="E52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53">
-        <v>1190</v>
-      </c>
-      <c r="E53" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>106</v>
-      </c>
-      <c r="B54" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54">
-        <v>990</v>
-      </c>
-      <c r="E54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55">
-        <v>1290</v>
-      </c>
-      <c r="E55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56">
-        <v>900</v>
-      </c>
-      <c r="E56" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57">
-        <v>1190</v>
-      </c>
-      <c r="E57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58">
-        <v>740</v>
-      </c>
-      <c r="E58" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>111</v>
-      </c>
-      <c r="B59" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59">
-        <v>1200</v>
-      </c>
-      <c r="E59" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60">
-        <v>1820</v>
-      </c>
-      <c r="E60" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61">
-        <v>1190</v>
-      </c>
-      <c r="E61" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62">
-        <v>1190</v>
-      </c>
-      <c r="E62" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>115</v>
-      </c>
-      <c r="B63" t="s">
-        <v>86</v>
-      </c>
-      <c r="C63">
-        <v>1600</v>
-      </c>
-      <c r="E63" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>116</v>
-      </c>
-      <c r="B64" t="s">
-        <v>86</v>
-      </c>
-      <c r="C64">
-        <v>1600</v>
-      </c>
-      <c r="E64" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>117</v>
-      </c>
-      <c r="B65" t="s">
-        <v>86</v>
-      </c>
-      <c r="C65">
-        <v>1600</v>
-      </c>
-      <c r="E65" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66">
-        <v>1799</v>
-      </c>
-      <c r="E66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>119</v>
-      </c>
-      <c r="B67" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67">
-        <v>990</v>
-      </c>
-      <c r="E67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>120</v>
-      </c>
-      <c r="B68" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68">
-        <v>990</v>
-      </c>
-      <c r="E68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>121</v>
-      </c>
-      <c r="B69" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69">
-        <v>1990</v>
-      </c>
-      <c r="E69" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>122</v>
-      </c>
-      <c r="B70" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70">
-        <v>999</v>
-      </c>
-      <c r="E70" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>123</v>
-      </c>
-      <c r="B71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C71">
-        <v>999</v>
-      </c>
-      <c r="E71" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>138</v>
-      </c>
-      <c r="B72" t="s">
-        <v>144</v>
-      </c>
-      <c r="C72">
-        <v>1150</v>
-      </c>
-      <c r="E72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" t="s">
-        <v>145</v>
-      </c>
-      <c r="C73">
-        <v>1200</v>
-      </c>
-      <c r="E73" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" t="s">
-        <v>146</v>
-      </c>
-      <c r="C74">
-        <v>1150</v>
-      </c>
-      <c r="E74" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>141</v>
-      </c>
-      <c r="B75" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75">
-        <v>1200</v>
-      </c>
-      <c r="E75" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" t="s">
-        <v>148</v>
-      </c>
-      <c r="C76">
-        <v>1150</v>
-      </c>
-      <c r="E76" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>143</v>
-      </c>
-      <c r="B77" t="s">
-        <v>149</v>
-      </c>
-      <c r="C77">
-        <v>1150</v>
-      </c>
-      <c r="E77" t="s">
-        <v>58</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="ae7cfdcc-53b0-4487-bc1f-feac62084570" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="ae7cfdcc-53b0-4487-bc1f-feac62084570" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2823,6 +3349,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A96F1F-4671-425A-901E-4E9D3728F5E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EA86CC4-3158-4E56-AB70-417726578CF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2834,14 +3368,6 @@
     <ds:schemaRef ds:uri="ae7cfdcc-53b0-4487-bc1f-feac62084570"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75A96F1F-4671-425A-901E-4E9D3728F5E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>